<commit_message>
ASC Automation- pages and test classes for account and territories
</commit_message>
<xml_diff>
--- a/testdata/MasterData_ASC_STAGE.xlsx
+++ b/testdata/MasterData_ASC_STAGE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stryker-my.sharepoint.com/personal/sanjay_dewrari_stryker_com/Documents/Automation Proj Template-Stryker/ProjectTemplate/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stryker_Automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="588" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="340" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
   <si>
     <t>Run</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Sr.no</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -52,84 +49,79 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>shrey.jain@stryker.com.stage</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>AccountManagement_TC_01</t>
   </si>
   <si>
-    <t>stryker12345</t>
+    <t>TestCase_Title</t>
+  </si>
+  <si>
+    <t>Profile|Role</t>
+  </si>
+  <si>
+    <t>NewTestCaseID</t>
+  </si>
+  <si>
+    <t>164716 - Account Setup</t>
+  </si>
+  <si>
+    <t>anshuman.sharma@stryker.com.uat</t>
+  </si>
+  <si>
+    <t>welcome12#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">164723 - This is to validate fields in the ASC Account Page Layout </t>
+  </si>
+  <si>
+    <t>AccountAndTerritories_227835_TC_01</t>
+  </si>
+  <si>
+    <t>AccountAndTerritories_227836_TC_02</t>
+  </si>
+  <si>
+    <t>AccountAndTerritories_227837_TC_03</t>
+  </si>
+  <si>
+    <t>AccountAndTerritories_227838_TC_04</t>
+  </si>
+  <si>
+    <t>AccountAndTerritories_227839_TC_05</t>
+  </si>
+  <si>
+    <t>AccountAndTerritories_227845_TC_05</t>
+  </si>
+  <si>
+    <t>AccountAndTerritories_227847_TC_06</t>
+  </si>
+  <si>
+    <t>AccountAndTerritories_227848_TC_07</t>
+  </si>
+  <si>
+    <t>AccountAndTerritories_227849_TC_08</t>
+  </si>
+  <si>
+    <t>AccountAndTerritories_227855_TC_09</t>
+  </si>
+  <si>
+    <t>AccountAndTerritories_227856_TC_10</t>
+  </si>
+  <si>
+    <t>AccountAndTerritories_227858_TC_11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -196,6 +188,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -237,41 +236,41 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -280,7 +279,92 @@
     <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -553,16 +637,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -570,24 +655,24 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -595,13 +680,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="4"/>
@@ -625,112 +710,367 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.6328125" style="1" collapsed="1"/>
-    <col min="2" max="2" width="36.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.6328125" style="1" collapsed="1"/>
-    <col min="4" max="6" width="8.6328125" style="1"/>
-    <col min="7" max="16384" width="8.6328125" style="1" collapsed="1"/>
+    <col min="1" max="1" width="8.5703125" style="1" collapsed="1"/>
+    <col min="2" max="2" width="53.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="44.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="1"/>
+    <col min="7" max="16384" width="8.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="D1" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="17"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="20"/>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="9"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="9"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="7"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="7"/>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="11">
+        <v>227835</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="11">
+        <v>227836</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="11">
+        <v>227837</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="11">
+        <v>227838</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="11">
+        <v>227839</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="11">
+        <v>227840</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="11">
+        <v>227841</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="11">
+        <v>227842</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="11">
+        <v>227843</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="11">
+        <v>227844</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="11">
+        <v>227845</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="11">
+        <v>227846</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="D15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="11">
+        <v>227847</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="D16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="11">
+        <v>227848</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="D17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="11">
+        <v>227849</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="D18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="11">
+        <v>227850</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="D19" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="11">
+        <v>227851</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="D20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="11">
+        <v>227852</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="D21" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="11">
+        <v>227853</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:A21">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A21">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>